<commit_message>
soa and doc updates
</commit_message>
<xml_diff>
--- a/Docs/Badge Order Tracking.xlsx
+++ b/Docs/Badge Order Tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlfugate/Documents/GitHub/Project-Gimli/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tier3tech-my.sharepoint.com/personal/kevin_badgepirates_com/Documents/Badges/Project-Gimli/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969BC990-212E-314E-9A68-405BCF54CF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{969BC990-212E-314E-9A68-405BCF54CF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFCE3EA4-99C4-4E3E-889B-D9BED7F542DA}"/>
   <bookViews>
-    <workbookView xWindow="16180" yWindow="11500" windowWidth="38880" windowHeight="26500" xr2:uid="{B1BD5E10-8107-EA4B-AC68-BCA33827D9A0}"/>
+    <workbookView xWindow="9768" yWindow="948" windowWidth="32856" windowHeight="18648" xr2:uid="{B1BD5E10-8107-EA4B-AC68-BCA33827D9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>Badge Order Tracking</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>PCB</t>
-  </si>
-  <si>
-    <t>Speaker</t>
   </si>
   <si>
     <t>QTY</t>
@@ -134,10 +131,37 @@
     <t>EC11 Rotary Encoders</t>
   </si>
   <si>
-    <t>ESP32-S2</t>
-  </si>
-  <si>
     <t>Kevin</t>
+  </si>
+  <si>
+    <t>Kids Badge</t>
+  </si>
+  <si>
+    <t>BP</t>
+  </si>
+  <si>
+    <t>1Z7759450315420785</t>
+  </si>
+  <si>
+    <t>1Z7759450315381425</t>
+  </si>
+  <si>
+    <t>ESP32-S2, LED's</t>
+  </si>
+  <si>
+    <t>Kids Badge - IR TX/RX, Transisters</t>
+  </si>
+  <si>
+    <t>Solder Village SAO, Poster SAO</t>
+  </si>
+  <si>
+    <t>400+</t>
+  </si>
+  <si>
+    <t>Sponsor</t>
+  </si>
+  <si>
+    <t>Sponsor SOA's, Speaker Add (10)</t>
   </si>
 </sst>
 </file>
@@ -215,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -251,6 +275,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,29 +659,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32386E0F-356F-5A49-9A2E-A7B7341B96CB}">
-  <dimension ref="A3:I35"/>
+  <dimension ref="A3:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="171" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="16.19921875" style="4" customWidth="1"/>
     <col min="2" max="2" width="56.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="10.83203125" style="4"/>
+    <col min="3" max="6" width="10.796875" style="4"/>
     <col min="7" max="7" width="27.5" style="4" customWidth="1"/>
-    <col min="8" max="9" width="10.83203125" style="4"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="9" width="10.796875" style="4"/>
+    <col min="10" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" ht="37" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="36.6" x14ac:dyDescent="0.7">
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -665,7 +693,7 @@
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -673,16 +701,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>6</v>
@@ -694,18 +722,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C9" s="10">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -713,226 +741,330 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4">
         <v>25</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1409.25</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="C11" s="6">
+        <v>405</v>
+      </c>
       <c r="D11" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C12" s="4">
+        <v>40</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="C13" s="6">
+        <v>30</v>
+      </c>
       <c r="D13" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4">
         <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="C15" s="6">
+        <v>15</v>
+      </c>
       <c r="D15" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="4">
+        <v>50</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="E16" s="4">
+        <v>315.05</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="6">
+        <v>50</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="6">
+        <v>203.51</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1322.27</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="6">
+        <v>500</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="6">
+        <v>178.59</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="6">
+        <v>2854852803</v>
+      </c>
+      <c r="H19" s="11">
+        <v>44816</v>
+      </c>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="4">
-        <v>1322.27</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="6">
-        <v>500</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="6">
-        <v>178.59</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="6">
-        <v>2854852803</v>
-      </c>
-      <c r="H17" s="11">
-        <v>44816</v>
-      </c>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="4">
-        <v>450</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="4">
-        <v>608.54999999999995</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1281.03</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="C20" s="4">
         <v>450</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="4">
+        <v>608.54999999999995</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="D21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1281.03</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="4">
+        <v>450</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="4">
+        <v>3991.32</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="13">
+        <v>44811</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="6">
+        <v>100</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="6">
+        <v>90.39</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="11">
+        <v>44812</v>
+      </c>
       <c r="I23" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -943,7 +1075,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -954,7 +1086,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -965,7 +1097,7 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -976,7 +1108,7 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -987,7 +1119,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -998,8 +1130,20 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
     </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>